<commit_message>
Control statements and Array
</commit_message>
<xml_diff>
--- a/2024FEB_B6.xlsx
+++ b/2024FEB_B6.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>S.N.</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>User inputs and outputs: int, string with methods</t>
+  </si>
+  <si>
+    <t>Worked with previously done control statement practical works, arrays: int, string, sorting: asc, dec</t>
   </si>
 </sst>
 </file>
@@ -534,7 +537,9 @@
       <c r="B7" s="8">
         <v>45338</v>
       </c>
-      <c r="C7" s="9"/>
+      <c r="C7" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="7">

</xml_diff>

<commit_message>
Array sort and type conversion
</commit_message>
<xml_diff>
--- a/2024FEB_B6.xlsx
+++ b/2024FEB_B6.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>S.N.</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>Saturday : Holiday</t>
+  </si>
+  <si>
+    <t>Array sort and Type Conversion</t>
   </si>
 </sst>
 </file>
@@ -562,7 +565,9 @@
       <c r="B9" s="8">
         <v>45340</v>
       </c>
-      <c r="C9" s="9"/>
+      <c r="C9" s="9" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="7">

</xml_diff>

<commit_message>
New updates on Constructor
</commit_message>
<xml_diff>
--- a/2024FEB_B6.xlsx
+++ b/2024FEB_B6.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SCCSB6\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F4E37DD-2940-4FA8-A506-FF9384A8DBA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>S.N.</t>
   </si>
@@ -56,15 +62,18 @@
   </si>
   <si>
     <t>Syllabus explanation, Constructor and destructor</t>
+  </si>
+  <si>
+    <t>Parameterized constructor with user input, Constructor Overloading; different no of parameters</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode=",,"/>
-    <numFmt numFmtId="165" formatCode="dddd, mmmm dd, yyyy"/>
+    <numFmt numFmtId="164" formatCode="\,"/>
+    <numFmt numFmtId="165" formatCode="dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -97,7 +106,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFff0000"/>
+        <fgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
   </fills>
@@ -129,52 +138,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -185,10 +197,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -226,71 +238,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -318,7 +330,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -341,11 +353,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -354,13 +366,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -370,7 +382,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -379,7 +391,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -388,7 +400,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -396,10 +408,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -464,22 +476,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="10" width="4.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="11" width="28.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="80.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="4.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="90.42578125" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -490,7 +504,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row r="2" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -501,7 +515,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row r="3" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -512,7 +526,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row r="4" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -523,7 +537,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row r="5" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -534,7 +548,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row r="6" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -545,7 +559,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row r="7" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -556,7 +570,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row r="8" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -567,7 +581,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row r="9" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -578,7 +592,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+    <row r="10" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -589,7 +603,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+    <row r="11" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -600,7 +614,7 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+    <row r="12" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>11</v>
       </c>
@@ -611,16 +625,18 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+    <row r="13" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>12</v>
       </c>
       <c r="B13" s="8">
         <v>45344</v>
       </c>
-      <c r="C13" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+      <c r="C13" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>13</v>
       </c>
@@ -629,7 +645,7 @@
       </c>
       <c r="C14" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25">
+    <row r="15" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>14</v>
       </c>
@@ -637,6 +653,216 @@
         <v>45346</v>
       </c>
       <c r="C15" s="9"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="8">
+        <v>45347</v>
+      </c>
+      <c r="C16" s="9"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="8">
+        <v>45348</v>
+      </c>
+      <c r="C17" s="9"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="8">
+        <v>45349</v>
+      </c>
+      <c r="C18" s="9"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="8">
+        <v>45350</v>
+      </c>
+      <c r="C19" s="9"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="8">
+        <v>45351</v>
+      </c>
+      <c r="C20" s="9"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="8">
+        <v>45352</v>
+      </c>
+      <c r="C21" s="9"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="8">
+        <v>45353</v>
+      </c>
+      <c r="C22" s="9"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="8">
+        <v>45354</v>
+      </c>
+      <c r="C23" s="9"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="8">
+        <v>45355</v>
+      </c>
+      <c r="C24" s="9"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="8">
+        <v>45356</v>
+      </c>
+      <c r="C25" s="9"/>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="8">
+        <v>45357</v>
+      </c>
+      <c r="C26" s="9"/>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="8">
+        <v>45358</v>
+      </c>
+      <c r="C27" s="9"/>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="8">
+        <v>45359</v>
+      </c>
+      <c r="C28" s="9"/>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="8">
+        <v>45360</v>
+      </c>
+      <c r="C29" s="9"/>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="8">
+        <v>45361</v>
+      </c>
+      <c r="C30" s="9"/>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="8">
+        <v>45362</v>
+      </c>
+      <c r="C31" s="9"/>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="8">
+        <v>45363</v>
+      </c>
+      <c r="C32" s="9"/>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="8">
+        <v>45364</v>
+      </c>
+      <c r="C33" s="9"/>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="8">
+        <v>45365</v>
+      </c>
+      <c r="C34" s="9"/>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="8">
+        <v>45366</v>
+      </c>
+      <c r="C35" s="9"/>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="8">
+        <v>45367</v>
+      </c>
+      <c r="C36" s="9"/>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="8">
+        <v>45368</v>
+      </c>
+      <c r="C37" s="9"/>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="8">
+        <v>45369</v>
+      </c>
+      <c r="C38" s="9"/>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="8">
+        <v>45370</v>
+      </c>
+      <c r="C39" s="9"/>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="8">
+        <v>45371</v>
+      </c>
+      <c r="C40" s="9"/>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="8">
+        <v>45372</v>
+      </c>
+      <c r="C41" s="9"/>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="8">
+        <v>45373</v>
+      </c>
+      <c r="C42" s="9"/>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="8">
+        <v>45374</v>
+      </c>
+      <c r="C43" s="9"/>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="8">
+        <v>45375</v>
+      </c>
+      <c r="C44" s="9"/>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="8">
+        <v>45376</v>
+      </c>
+      <c r="C45" s="9"/>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="8">
+        <v>45377</v>
+      </c>
+      <c r="C46" s="9"/>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="8">
+        <v>45378</v>
+      </c>
+      <c r="C47" s="9"/>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B48" s="8">
+        <v>45379</v>
+      </c>
+      <c r="C48" s="9"/>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="8">
+        <v>45380</v>
+      </c>
+      <c r="C49" s="9"/>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" s="8">
+        <v>45381</v>
+      </c>
+      <c r="C50" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New updates on Inheritance
</commit_message>
<xml_diff>
--- a/2024FEB_B6.xlsx
+++ b/2024FEB_B6.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>S.N.</t>
   </si>
@@ -77,6 +77,12 @@
   </si>
   <si>
     <t>Enumeration</t>
+  </si>
+  <si>
+    <t>Partial Classes</t>
+  </si>
+  <si>
+    <t>Static Classes, Static Properties, Inheritance</t>
   </si>
 </sst>
 </file>
@@ -87,7 +93,7 @@
     <numFmt numFmtId="164" formatCode=",,"/>
     <numFmt numFmtId="165" formatCode="dddd, mmmm dd, yyyy"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,12 +111,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -191,11 +191,11 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -731,21 +731,27 @@
       <c r="B21" s="8">
         <v>45352</v>
       </c>
-      <c r="C21" s="9"/>
+      <c r="C21" s="9" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="10"/>
       <c r="B22" s="8">
         <v>45353</v>
       </c>
-      <c r="C22" s="9"/>
+      <c r="C22" s="9" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="10"/>
       <c r="B23" s="8">
         <v>45354</v>
       </c>
-      <c r="C23" s="9"/>
+      <c r="C23" s="9" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="10"/>

</xml_diff>

<commit_message>
Sealed Class, Interface and multiple inheritace with class problem scenario
</commit_message>
<xml_diff>
--- a/2024FEB_B6.xlsx
+++ b/2024FEB_B6.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>S.N.</t>
   </si>
@@ -83,6 +83,27 @@
   </si>
   <si>
     <t>Static Classes, Static Properties, Inheritance</t>
+  </si>
+  <si>
+    <t>Polymorphism</t>
+  </si>
+  <si>
+    <t xml:space="preserve">College holiday : due to untimely demise of a Student </t>
+  </si>
+  <si>
+    <t>Leave, External Examiner</t>
+  </si>
+  <si>
+    <t>Practival Exam VIVA Fifth Semester</t>
+  </si>
+  <si>
+    <t>Shivaratri : Holiday</t>
+  </si>
+  <si>
+    <t>Sealed Class and Interface</t>
+  </si>
+  <si>
+    <t>Gyalpo Lhosar : Holiday</t>
   </si>
 </sst>
 </file>
@@ -758,79 +779,95 @@
       <c r="B24" s="8">
         <v>45355</v>
       </c>
-      <c r="C24" s="9"/>
+      <c r="C24" s="9" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="10"/>
       <c r="B25" s="8">
         <v>45356</v>
       </c>
-      <c r="C25" s="9"/>
+      <c r="C25" s="9" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="10"/>
       <c r="B26" s="8">
         <v>45357</v>
       </c>
-      <c r="C26" s="9"/>
+      <c r="C26" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="10"/>
       <c r="B27" s="8">
         <v>45358</v>
       </c>
-      <c r="C27" s="9"/>
+      <c r="C27" s="9" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="10"/>
       <c r="B28" s="8">
         <v>45359</v>
       </c>
-      <c r="C28" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+      <c r="C28" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="10"/>
       <c r="B29" s="8">
         <v>45360</v>
       </c>
-      <c r="C29" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+      <c r="C29" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="10"/>
       <c r="B30" s="8">
         <v>45361</v>
       </c>
-      <c r="C30" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+      <c r="C30" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
       <c r="A31" s="10"/>
       <c r="B31" s="8">
         <v>45362</v>
       </c>
-      <c r="C31" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+      <c r="C31" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
       <c r="A32" s="10"/>
       <c r="B32" s="8">
         <v>45363</v>
       </c>
       <c r="C32" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
       <c r="A33" s="10"/>
       <c r="B33" s="8">
         <v>45364</v>
       </c>
       <c r="C33" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
       <c r="A34" s="10"/>
       <c r="B34" s="8">
         <v>45365</v>
       </c>
       <c r="C34" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
       <c r="A35" s="10"/>
       <c r="B35" s="8">
         <v>45366</v>

</xml_diff>

<commit_message>
Interface with c/w solution
</commit_message>
<xml_diff>
--- a/2024FEB_B6.xlsx
+++ b/2024FEB_B6.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>S.N.</t>
   </si>
@@ -104,6 +104,12 @@
   </si>
   <si>
     <t>Gyalpo Lhosar : Holiday</t>
+  </si>
+  <si>
+    <t>Class break due to a Program, Student's special request</t>
+  </si>
+  <si>
+    <t>Interface</t>
   </si>
 </sst>
 </file>
@@ -851,14 +857,18 @@
       <c r="B32" s="8">
         <v>45363</v>
       </c>
-      <c r="C32" s="9"/>
+      <c r="C32" s="9" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
       <c r="A33" s="10"/>
       <c r="B33" s="8">
         <v>45364</v>
       </c>
-      <c r="C33" s="9"/>
+      <c r="C33" s="9" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
       <c r="A34" s="10"/>
@@ -874,42 +884,42 @@
       </c>
       <c r="C35" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
       <c r="A36" s="10"/>
       <c r="B36" s="8">
         <v>45367</v>
       </c>
       <c r="C36" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
       <c r="A37" s="10"/>
       <c r="B37" s="8">
         <v>45368</v>
       </c>
       <c r="C37" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
       <c r="A38" s="10"/>
       <c r="B38" s="8">
         <v>45369</v>
       </c>
       <c r="C38" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
       <c r="A39" s="10"/>
       <c r="B39" s="8">
         <v>45370</v>
       </c>
       <c r="C39" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
       <c r="A40" s="10"/>
       <c r="B40" s="8">
         <v>45371</v>
       </c>
       <c r="C40" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
       <c r="A41" s="10"/>
       <c r="B41" s="8">
         <v>45372</v>

</xml_diff>

<commit_message>
abstract class and methods
</commit_message>
<xml_diff>
--- a/2024FEB_B6.xlsx
+++ b/2024FEB_B6.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>S.N.</t>
   </si>
@@ -110,6 +110,15 @@
   </si>
   <si>
     <t>Interface</t>
+  </si>
+  <si>
+    <t>Virtual Methods and Abstract Class and Methods</t>
+  </si>
+  <si>
+    <t>Abstract Class and Methods</t>
+  </si>
+  <si>
+    <t>Holiday : Saturday</t>
   </si>
 </sst>
 </file>
@@ -875,21 +884,27 @@
       <c r="B34" s="8">
         <v>45365</v>
       </c>
-      <c r="C34" s="9"/>
+      <c r="C34" s="9" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
       <c r="A35" s="10"/>
       <c r="B35" s="8">
         <v>45366</v>
       </c>
-      <c r="C35" s="9"/>
+      <c r="C35" s="9" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
       <c r="A36" s="10"/>
       <c r="B36" s="8">
         <v>45367</v>
       </c>
-      <c r="C36" s="9"/>
+      <c r="C36" s="9" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
       <c r="A37" s="10"/>
@@ -926,21 +941,21 @@
       </c>
       <c r="C41" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
       <c r="A42" s="10"/>
       <c r="B42" s="8">
         <v>45373</v>
       </c>
       <c r="C42" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
       <c r="A43" s="10"/>
       <c r="B43" s="8">
         <v>45374</v>
       </c>
       <c r="C43" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
       <c r="A44" s="10"/>
       <c r="B44" s="8">
         <v>45375</v>

</xml_diff>